<commit_message>
SelectGermlineVariants & other stuff
</commit_message>
<xml_diff>
--- a/docs/mutant expression pipeline.xlsx
+++ b/docs/mutant expression pipeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="162">
   <si>
     <t>Generated By</t>
   </si>
@@ -461,9 +461,6 @@
     <t>GenerateScatterGraphs, RegionalExpression</t>
   </si>
   <si>
-    <t>ExpressionDistribution, GenerateScatterGraphs, RegionalExpression, ExpressionNearMutations</t>
-  </si>
-  <si>
     <t>ExpressionNearMutations</t>
   </si>
   <si>
@@ -492,6 +489,27 @@
   </si>
   <si>
     <t>experiments.txt, maf, *.regional_expression.txt, &lt;gene&gt;_unfiltered_counts.txt</t>
+  </si>
+  <si>
+    <t>&lt;analysis&gt;.selectedVariants</t>
+  </si>
+  <si>
+    <t>High quality germline SNPs selected to measure ASE</t>
+  </si>
+  <si>
+    <t>SelectGermlineVariants</t>
+  </si>
+  <si>
+    <t>\tcga\&lt;disease&gt;\normal\dna\&lt;analysis-id&gt;\&lt;analysis-id&gt;.selectedVariants</t>
+  </si>
+  <si>
+    <t>*.vcf, experiments.txt</t>
+  </si>
+  <si>
+    <t>ExpressionDistribution, GenerateScatterGraphs, RegionalExpression, ExpressionNearMutations, SelectGermlineVariants</t>
+  </si>
+  <si>
+    <t>ExpressionMetadata, SelectGermlineVariants</t>
   </si>
 </sst>
 </file>
@@ -824,7 +842,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +907,7 @@
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1342,7 +1360,7 @@
         <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1368,7 +1386,7 @@
         <v>138</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1628,12 +1646,12 @@
         <v>143</v>
       </c>
       <c r="I31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
         <v>49</v>
@@ -1642,21 +1660,21 @@
         <v>133</v>
       </c>
       <c r="D32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
         <v>149</v>
       </c>
-      <c r="E32" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" t="s">
-        <v>150</v>
-      </c>
       <c r="G32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
@@ -1665,23 +1683,43 @@
         <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E33" t="s">
         <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" t="s">
         <v>121</v>
       </c>
       <c r="I33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
+      <c r="A34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>

</xml_diff>

<commit_message>
Make SelectGermlineVariants only choose those with reads; fix RegionalExpression
</commit_message>
<xml_diff>
--- a/docs/mutant expression pipeline.xlsx
+++ b/docs/mutant expression pipeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="192">
   <si>
     <t>Generated By</t>
   </si>
@@ -497,9 +497,6 @@
     <t>SelectGermlineVariants</t>
   </si>
   <si>
-    <t>*.vcf, experiments.txt</t>
-  </si>
-  <si>
     <t>ExpressionDistribution, GenerateScatterGraphs, RegionalExpression, ExpressionNearMutations, SelectGermlineVariants</t>
   </si>
   <si>
@@ -543,6 +540,66 @@
   </si>
   <si>
     <t>*.annotatedSelectedVariants</t>
+  </si>
+  <si>
+    <t>ExpressionDistribution, SelectGermlineVariants, RegionalExpression</t>
+  </si>
+  <si>
+    <t>*.vcf, experiments.txt, allcount (DNA &amp; RNA)</t>
+  </si>
+  <si>
+    <t>&lt;analysis&gt;.annotatedSelectedVariants.txt</t>
+  </si>
+  <si>
+    <t>selected variants + RNA &amp; DNA read counts at the variant locus</t>
+  </si>
+  <si>
+    <t>\tcga\&lt;disease&gt;\tumor\normal\{wgs|wxs}\&lt;analysis-id&gt;\&lt;analysis-id&gt;.annotatedSelectedVariants</t>
+  </si>
+  <si>
+    <t>indices, *.selectedVariants, *.readsAtSelectedVariants</t>
+  </si>
+  <si>
+    <t>ExpressionByMutationCount</t>
+  </si>
+  <si>
+    <t>\temp\expression\</t>
+  </si>
+  <si>
+    <t>&lt;gene&gt;_lines.txt</t>
+  </si>
+  <si>
+    <t>\temp\expression\RegionalExpressionByGene</t>
+  </si>
+  <si>
+    <t>Normalized expression level around genes &amp; mutation count for each tumor</t>
+  </si>
+  <si>
+    <t>Final results</t>
+  </si>
+  <si>
+    <t>experiments.txt, *.gene_expression.txt, &lt;gene&gt;.unfiltered_counts.txt</t>
+  </si>
+  <si>
+    <t>ExpressionDistributionByMutationCount</t>
+  </si>
+  <si>
+    <t>p values for expression around genes by mutation count</t>
+  </si>
+  <si>
+    <t>&lt;gene&gt;_allele_specific_lines.txt</t>
+  </si>
+  <si>
+    <t>AlleleSpecificExpressionDistributionByMutationCount</t>
+  </si>
+  <si>
+    <t>Normalized allele-specific expression level around genes &amp; mutation count for each tumor</t>
+  </si>
+  <si>
+    <t>p values for allele-specific expression around genes by mutation count</t>
+  </si>
+  <si>
+    <t>experiments.txt, *.allele_specific_gene_expression.txt, &lt;gene&gt;.unfiltered_counts.txt</t>
   </si>
 </sst>
 </file>
@@ -872,21 +929,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="71.5703125" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" customWidth="1"/>
-    <col min="6" max="6" width="75.42578125" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" customWidth="1"/>
+    <col min="6" max="6" width="88.140625" customWidth="1"/>
+    <col min="7" max="7" width="77.140625" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="77.28515625" customWidth="1"/>
   </cols>
@@ -1318,7 +1375,7 @@
         <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1393,7 +1450,7 @@
         <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1419,7 +1476,7 @@
         <v>94</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1748,18 +1805,18 @@
         <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G34" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="I34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
@@ -1768,78 +1825,190 @@
         <v>133</v>
       </c>
       <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
         <v>160</v>
       </c>
-      <c r="E35" t="s">
-        <v>161</v>
-      </c>
       <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
         <v>163</v>
       </c>
-      <c r="G35" t="s">
-        <v>164</v>
-      </c>
       <c r="H35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>103</v>
+        <v>176</v>
+      </c>
+      <c r="G36" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" t="s">
         <v>169</v>
       </c>
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="E38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" t="s">
+        <v>170</v>
+      </c>
+      <c r="G38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D37" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" t="s">
-        <v>171</v>
-      </c>
-      <c r="G37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
+      <c r="D39" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" t="s">
+        <v>181</v>
+      </c>
+      <c r="G39" t="s">
+        <v>184</v>
+      </c>
+      <c r="I39" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="2"/>
+      <c r="A40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" t="s">
+        <v>186</v>
+      </c>
+      <c r="E40" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" t="s">
+        <v>184</v>
+      </c>
+      <c r="I40" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
+      <c r="A41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" t="s">
+        <v>189</v>
+      </c>
+      <c r="E41" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" t="s">
+        <v>191</v>
+      </c>
+      <c r="I41" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
+      <c r="A42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" t="s">
+        <v>190</v>
+      </c>
+      <c r="E42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" t="s">
+        <v>191</v>
+      </c>
+      <c r="I42" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
@@ -1849,6 +2018,9 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
measure gene coverage started
</commit_message>
<xml_diff>
--- a/docs/mutant expression pipeline.xlsx
+++ b/docs/mutant expression pipeline.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="208">
   <si>
     <t>Generated By</t>
   </si>
@@ -236,24 +236,12 @@
     <t>Expression Metadata</t>
   </si>
   <si>
-    <t>allcount</t>
-  </si>
-  <si>
     <t>compressed text</t>
   </si>
   <si>
-    <t>RNA coverage of the genome</t>
-  </si>
-  <si>
     <t>allCount*.cmd</t>
   </si>
   <si>
-    <t>\tcga\&lt;disease&gt;\{tumor,normal}\rna\&lt;analysis-id&gt;\*.allcount.gz</t>
-  </si>
-  <si>
-    <t>existing allcount files, list of stored RNA BAMs</t>
-  </si>
-  <si>
     <t>RNA BAM</t>
   </si>
   <si>
@@ -633,6 +621,33 @@
   </si>
   <si>
     <t>The results for {allele specific} expression pan-cancer and per-cancer with p &lt; .01 after correction</t>
+  </si>
+  <si>
+    <t>&lt;analysis&gt;.gene_coverage.txt</t>
+  </si>
+  <si>
+    <t>The read coverage of the exons of each gene as a fraction of the coverage of all exons</t>
+  </si>
+  <si>
+    <t>\tcga\&lt;disease&gt;\tumor\{wgs,wxs}\&lt;analysis-id&gt;\&lt;analysis-id&gt;.gene_coverage.txt</t>
+  </si>
+  <si>
+    <t>allcount (tumor DNA)</t>
+  </si>
+  <si>
+    <t>&lt;analysis-id&gt;.allcount.gz</t>
+  </si>
+  <si>
+    <t>Read coverage of the genome</t>
+  </si>
+  <si>
+    <t>\tcga\&lt;disease&gt;\{tumor,normal}\{rna,wgs,wxs}\&lt;analysis-id&gt;\*.allcount.gz</t>
+  </si>
+  <si>
+    <t>existing allcount files, list of stored BAMs</t>
+  </si>
+  <si>
+    <t>MeasureGeneCoverage</t>
   </si>
 </sst>
 </file>
@@ -964,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +1004,7 @@
         <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1018,7 +1033,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1030,7 +1045,7 @@
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1041,7 +1056,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1064,7 +1079,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -1087,7 +1102,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1110,7 +1125,7 @@
         <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -1136,7 +1151,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -1148,7 +1163,7 @@
         <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1159,7 +1174,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -1171,7 +1186,7 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H8" t="s">
         <v>33</v>
@@ -1185,7 +1200,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -1203,7 +1218,7 @@
         <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1214,7 +1229,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
@@ -1232,7 +1247,7 @@
         <v>39</v>
       </c>
       <c r="I10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1243,7 +1258,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -1255,7 +1270,7 @@
         <v>47</v>
       </c>
       <c r="I11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1266,10 +1281,10 @@
         <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
@@ -1278,7 +1293,7 @@
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1289,7 +1304,7 @@
         <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
         <v>55</v>
@@ -1318,7 +1333,7 @@
         <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
         <v>60</v>
@@ -1367,7 +1382,7 @@
         <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
         <v>66</v>
@@ -1387,42 +1402,42 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>205</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>206</v>
       </c>
       <c r="I17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -1431,12 +1446,12 @@
         <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
@@ -1445,33 +1460,33 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
         <v>23</v>
@@ -1480,50 +1495,50 @@
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
         <v>87</v>
       </c>
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>90</v>
       </c>
-      <c r="F21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" t="s">
-        <v>94</v>
-      </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>23</v>
@@ -1532,24 +1547,24 @@
         <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
         <v>23</v>
@@ -1558,50 +1573,50 @@
         <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>103</v>
-      </c>
-      <c r="G24" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E25" t="s">
         <v>23</v>
@@ -1610,516 +1625,536 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" t="s">
         <v>106</v>
       </c>
-      <c r="E26" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>103</v>
       </c>
-      <c r="G26" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" t="s">
-        <v>107</v>
-      </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s">
         <v>111</v>
       </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" t="s">
-        <v>115</v>
-      </c>
       <c r="I27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" t="s">
         <v>117</v>
       </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>121</v>
-      </c>
-      <c r="I28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" t="s">
         <v>121</v>
-      </c>
-      <c r="I29" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" t="s">
         <v>138</v>
       </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" t="s">
-        <v>139</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="I31" t="s">
         <v>140</v>
-      </c>
-      <c r="F31" t="s">
-        <v>141</v>
-      </c>
-      <c r="G31" t="s">
-        <v>142</v>
-      </c>
-      <c r="I31" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" t="s">
         <v>144</v>
       </c>
-      <c r="F32" t="s">
-        <v>148</v>
-      </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" t="s">
+        <v>169</v>
+      </c>
+      <c r="I34" t="s">
         <v>156</v>
-      </c>
-      <c r="F34" t="s">
-        <v>161</v>
-      </c>
-      <c r="G34" t="s">
-        <v>173</v>
-      </c>
-      <c r="I34" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" t="s">
         <v>159</v>
       </c>
-      <c r="E35" t="s">
-        <v>160</v>
-      </c>
-      <c r="F35" t="s">
-        <v>162</v>
-      </c>
-      <c r="G35" t="s">
-        <v>163</v>
-      </c>
       <c r="H35" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D36" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G36" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B37" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G38" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" t="s">
+        <v>177</v>
+      </c>
+      <c r="G39" t="s">
         <v>180</v>
       </c>
-      <c r="B39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" t="s">
-        <v>178</v>
-      </c>
-      <c r="F39" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" t="s">
-        <v>184</v>
-      </c>
       <c r="I39" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B40" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B41" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D41" t="s">
+        <v>184</v>
+      </c>
+      <c r="E41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" t="s">
+        <v>185</v>
+      </c>
+      <c r="I41" t="s">
         <v>188</v>
-      </c>
-      <c r="E41" t="s">
-        <v>178</v>
-      </c>
-      <c r="F41" t="s">
-        <v>181</v>
-      </c>
-      <c r="G41" t="s">
-        <v>189</v>
-      </c>
-      <c r="I41" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D42" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E42" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F42" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G42" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I42" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" t="s">
+        <v>187</v>
+      </c>
+      <c r="E43" t="s">
+        <v>188</v>
+      </c>
+      <c r="F43" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" t="s">
         <v>190</v>
       </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="I43" t="s">
         <v>191</v>
-      </c>
-      <c r="E43" t="s">
-        <v>192</v>
-      </c>
-      <c r="F43" t="s">
-        <v>193</v>
-      </c>
-      <c r="G43" t="s">
-        <v>194</v>
-      </c>
-      <c r="I43" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F44" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" t="s">
+        <v>198</v>
+      </c>
+      <c r="E45" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45" t="s">
+        <v>189</v>
+      </c>
+      <c r="G45" t="s">
+        <v>190</v>
+      </c>
+      <c r="I45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>200</v>
+      </c>
+      <c r="E46" t="s">
+        <v>207</v>
+      </c>
+      <c r="F46" t="s">
         <v>201</v>
       </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="G46" t="s">
         <v>202</v>
       </c>
-      <c r="E45" t="s">
-        <v>192</v>
-      </c>
-      <c r="F45" t="s">
-        <v>193</v>
-      </c>
-      <c r="G45" t="s">
-        <v>194</v>
-      </c>
-      <c r="I45" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>